<commit_message>
PROS-10209 CCPHL custom kpis
</commit_message>
<xml_diff>
--- a/Projects/CCPHL/Data/Template.xlsx
+++ b/Projects/CCPHL/Data/Template.xlsx
@@ -395,24 +395,24 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C39" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.5060728744939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.3765182186235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="29.8016194331984"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.96356275303644"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.5060728744939"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="6.64777327935223"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.2753036437247"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.1376518218623"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.9109311740891"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="16.6801619433198"/>
-    <col collapsed="false" hidden="false" max="1014" min="12" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1023" min="1015" style="4" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1014" min="12" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1023" min="1015" style="4" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,6 +830,7 @@
       <c r="F14" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="G14" s="0"/>
       <c r="H14" s="4" t="s">
         <v>17</v>
       </c>
@@ -862,6 +863,7 @@
       <c r="F15" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="G15" s="0"/>
       <c r="H15" s="4" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
PROS-10209- CCPHL scene_type update for custom kpis
</commit_message>
<xml_diff>
--- a/Projects/CCPHL/Data/Template.xlsx
+++ b/Projects/CCPHL/Data/Template.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">CPURITY_OWN_MANF_COOLER_SCENES_WHOLE_STORE</t>
   </si>
   <si>
-    <t xml:space="preserve">Two-door Cooler, One-door Cooler, CCV</t>
+    <t xml:space="preserve">One-door Cooler, Two-door Cooler, Open-curtain Chiller</t>
   </si>
   <si>
     <t xml:space="preserve">store</t>
@@ -236,7 +236,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,6 +291,10 @@
     </xf>
     <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -395,21 +399,21 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="bottomLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="43.1052631578947"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="1" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="16.9230769230769"/>
     <col collapsed="false" hidden="false" max="1014" min="12" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1023" min="1015" style="4" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.10526315789474"/>
@@ -711,8 +715,8 @@
       <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
       <c r="H10" s="4" t="s">
         <v>17</v>
       </c>
@@ -722,7 +726,7 @@
       <c r="J10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -742,16 +746,16 @@
       <c r="E11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
       <c r="H11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -769,8 +773,8 @@
       <c r="E12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="4" t="s">
         <v>17</v>
       </c>
@@ -780,7 +784,7 @@
       <c r="J12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -800,16 +804,16 @@
       <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
       <c r="H13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="18"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -840,7 +844,7 @@
       <c r="J14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -870,8 +874,8 @@
       <c r="I15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -904,7 +908,7 @@
       <c r="J16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -936,7 +940,7 @@
       <c r="I17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="18"/>
+      <c r="K17" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>